<commit_message>
Added Hackathon route for editing event with dynamic fields
</commit_message>
<xml_diff>
--- a/Event.xlsx
+++ b/Event.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="75">
   <si>
     <t>event_name</t>
   </si>
@@ -40,27 +40,42 @@
     <t>sponsorship_amount</t>
   </si>
   <si>
-    <t>Youth</t>
-  </si>
-  <si>
-    <t>National Centre for Biological Sciences</t>
-  </si>
-  <si>
-    <t>345</t>
-  </si>
-  <si>
-    <t>2019-02-14</t>
-  </si>
-  <si>
-    <t>2019-02-01</t>
+    <t>Call For Code 2020</t>
+  </si>
+  <si>
+    <t>Pravega Tech Fest 2020</t>
+  </si>
+  <si>
+    <t>NMIT</t>
+  </si>
+  <si>
+    <t>IISc</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>2020-10-20</t>
+  </si>
+  <si>
+    <t>2020-10-17</t>
+  </si>
+  <si>
+    <t>2020-10-16</t>
   </si>
   <si>
     <t>In Progress</t>
   </si>
   <si>
+    <t>Planned</t>
+  </si>
+  <si>
     <t>INR  10000</t>
   </si>
   <si>
+    <t>INR  50000</t>
+  </si>
+  <si>
     <t>main_event</t>
   </si>
   <si>
@@ -79,64 +94,85 @@
     <t>finaledate</t>
   </si>
   <si>
-    <t>technology</t>
+    <t>theme</t>
   </si>
   <si>
     <t>jury</t>
   </si>
   <si>
-    <t>additional_jury</t>
-  </si>
-  <si>
-    <t>winning_team_details</t>
-  </si>
-  <si>
-    <t>runnerup_team_details</t>
+    <t>team_name1</t>
+  </si>
+  <si>
+    <t>team_name2</t>
   </si>
   <si>
     <t>winning_team_profiles</t>
   </si>
   <si>
-    <t>codathon</t>
-  </si>
-  <si>
-    <t>National Law School of India University</t>
-  </si>
-  <si>
-    <t>12</t>
-  </si>
-  <si>
-    <t>21</t>
-  </si>
-  <si>
-    <t>11</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>2019-02-02</t>
-  </si>
-  <si>
-    <t>Java</t>
-  </si>
-  <si>
-    <t>[['roibin', 'IRL']]</t>
+    <t>test_hack1</t>
+  </si>
+  <si>
+    <t>Hack for Good</t>
+  </si>
+  <si>
+    <t>HackBout</t>
+  </si>
+  <si>
+    <t>500</t>
+  </si>
+  <si>
+    <t>250</t>
+  </si>
+  <si>
+    <t>100</t>
+  </si>
+  <si>
+    <t>10000</t>
+  </si>
+  <si>
+    <t>1500</t>
+  </si>
+  <si>
+    <t>400</t>
+  </si>
+  <si>
+    <t>2020-10-30</t>
+  </si>
+  <si>
+    <t>2020-10-19</t>
+  </si>
+  <si>
+    <t>AI</t>
+  </si>
+  <si>
+    <t>Blockchain</t>
+  </si>
+  <si>
+    <t>Cloud</t>
+  </si>
+  <si>
+    <t>[['Mr. Aditya', 'ISL']]</t>
+  </si>
+  <si>
+    <t>[['Dr. Dilip', 'ISL'], ['Dr. Aman', 'IRL'], ['Mr. Madhu', 'GBS'], ['Ms. Aditi', 'GTS']]</t>
+  </si>
+  <si>
+    <t>[['Mr. Aditya', 'ISL'], ['Mr. Ramesh', 'IRL']]</t>
   </si>
   <si>
     <t>Completed</t>
   </si>
   <si>
-    <t>xyz</t>
-  </si>
-  <si>
-    <t>pyteam</t>
-  </si>
-  <si>
-    <t>javateam</t>
-  </si>
-  <si>
-    <t>sfgdhdf</t>
+    <t>HACKERS</t>
+  </si>
+  <si>
+    <t>&lt;codeio&gt;</t>
+  </si>
+  <si>
+    <t>XYZ</t>
+  </si>
+  <si>
+    <t>ABC123</t>
   </si>
   <si>
     <t>bu</t>
@@ -151,6 +187,21 @@
     <t>box_location_feed</t>
   </si>
   <si>
+    <t xml:space="preserve">AI For Everyone </t>
+  </si>
+  <si>
+    <t>GBS</t>
+  </si>
+  <si>
+    <t>SME_NAME</t>
+  </si>
+  <si>
+    <t>BOX LOC ATTENDEE</t>
+  </si>
+  <si>
+    <t>BOX LOC FEEDBACK</t>
+  </si>
+  <si>
     <t>sur_topic_name</t>
   </si>
   <si>
@@ -191,78 +242,6 @@
   </si>
   <si>
     <t>project_url</t>
-  </si>
-  <si>
-    <t>software production</t>
-  </si>
-  <si>
-    <t>asfdgf</t>
-  </si>
-  <si>
-    <t>devlopment</t>
-  </si>
-  <si>
-    <t>Amit kumar</t>
-  </si>
-  <si>
-    <t>['Amit kumar']</t>
-  </si>
-  <si>
-    <t>['Amit kumar', 'manoj', 'manoj', 'akjsdnglk']</t>
-  </si>
-  <si>
-    <t>['Amit kumar', 'manoj', 'akjsdnglk', 'kjnfslkn', 'bfdkjnaslk']</t>
-  </si>
-  <si>
-    <t>['Amit kumar', 'manoj', 'kjnfslkn', 'akjsdnglk', 'kjnfslkn']</t>
-  </si>
-  <si>
-    <t>python</t>
-  </si>
-  <si>
-    <t>2019-02-07</t>
-  </si>
-  <si>
-    <t>2019-02-12</t>
-  </si>
-  <si>
-    <t>2019-02-11</t>
-  </si>
-  <si>
-    <t>2019-02-13</t>
-  </si>
-  <si>
-    <t>2019-02-06</t>
-  </si>
-  <si>
-    <t>2019-02-08</t>
-  </si>
-  <si>
-    <t>2019-02-09</t>
-  </si>
-  <si>
-    <t>Rejected</t>
-  </si>
-  <si>
-    <t>Approved</t>
-  </si>
-  <si>
-    <t>bangaluru</t>
-  </si>
-  <si>
-    <t>delhi</t>
-  </si>
-  <si>
-    <t>jsfdnlknd</t>
-  </si>
-  <si>
-    <t>example.com</t>
-  </si>
-  <si>
-    <t>sdkdnvsks.com</t>
-  </si>
-  <si>
-    <t>kjnjds.com</t>
   </si>
 </sst>
 </file>
@@ -620,7 +599,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -657,22 +636,48 @@
         <v>7</v>
       </c>
       <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
         <v>8</v>
       </c>
-      <c r="D2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="C3" t="s">
         <v>10</v>
       </c>
-      <c r="F2" t="s">
+      <c r="D3" t="s">
         <v>11</v>
       </c>
-      <c r="G2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H2" t="s">
+      <c r="E3" t="s">
         <v>13</v>
+      </c>
+      <c r="F3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -682,18 +687,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:R2"/>
+  <dimension ref="A1:Q4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:18">
+    <row r="1" spans="1:17">
       <c r="B1" s="1" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1</v>
@@ -702,13 +707,13 @@
         <v>2</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>4</v>
@@ -717,31 +722,28 @@
         <v>3</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="N1" s="1" t="s">
         <v>5</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:18">
+    <row r="2" spans="1:17">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -749,52 +751,155 @@
         <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="D2" t="s">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="E2" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="F2" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="G2" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="H2" t="s">
+        <v>38</v>
+      </c>
+      <c r="I2" t="s">
+        <v>39</v>
+      </c>
+      <c r="J2" t="s">
+        <v>39</v>
+      </c>
+      <c r="K2" t="s">
+        <v>39</v>
+      </c>
+      <c r="L2" t="s">
+        <v>41</v>
+      </c>
+      <c r="M2" t="s">
+        <v>44</v>
+      </c>
+      <c r="N2" t="s">
+        <v>15</v>
+      </c>
+      <c r="O2" t="s">
+        <v>48</v>
+      </c>
+      <c r="P2" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
         <v>31</v>
       </c>
-      <c r="I2" t="s">
+      <c r="D3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" t="s">
+        <v>34</v>
+      </c>
+      <c r="F3">
+        <v>1200</v>
+      </c>
+      <c r="G3">
+        <v>350</v>
+      </c>
+      <c r="H3">
+        <v>50</v>
+      </c>
+      <c r="I3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J3" t="s">
+        <v>14</v>
+      </c>
+      <c r="K3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L3" t="s">
+        <v>42</v>
+      </c>
+      <c r="M3" t="s">
+        <v>45</v>
+      </c>
+      <c r="N3" t="s">
+        <v>47</v>
+      </c>
+      <c r="O3" t="s">
+        <v>48</v>
+      </c>
+      <c r="P3" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
         <v>32</v>
       </c>
-      <c r="J2" t="s">
-        <v>10</v>
-      </c>
-      <c r="K2" t="s">
-        <v>10</v>
-      </c>
-      <c r="L2" t="s">
-        <v>33</v>
-      </c>
-      <c r="M2" t="s">
-        <v>34</v>
-      </c>
-      <c r="N2" t="s">
+      <c r="D4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" t="s">
         <v>35</v>
       </c>
-      <c r="O2" t="s">
-        <v>36</v>
-      </c>
-      <c r="P2" t="s">
-        <v>37</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>38</v>
-      </c>
-      <c r="R2" t="s">
-        <v>39</v>
+      <c r="F4">
+        <v>900</v>
+      </c>
+      <c r="G4">
+        <v>250</v>
+      </c>
+      <c r="H4">
+        <v>50</v>
+      </c>
+      <c r="I4" t="s">
+        <v>14</v>
+      </c>
+      <c r="J4" t="s">
+        <v>40</v>
+      </c>
+      <c r="K4" t="s">
+        <v>13</v>
+      </c>
+      <c r="L4" t="s">
+        <v>43</v>
+      </c>
+      <c r="M4" t="s">
+        <v>46</v>
+      </c>
+      <c r="N4" t="s">
+        <v>47</v>
+      </c>
+      <c r="O4" t="s">
+        <v>49</v>
+      </c>
+      <c r="P4" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -804,15 +909,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:M1"/>
+  <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="2:13">
+    <row r="1" spans="1:13">
       <c r="B1" s="1" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
@@ -833,19 +938,60 @@
         <v>3</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>40</v>
+        <v>52</v>
       </c>
       <c r="K1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F2" t="s">
+        <v>47</v>
+      </c>
+      <c r="G2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I2" t="s">
         <v>41</v>
       </c>
-      <c r="L1" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>43</v>
+      <c r="J2" t="s">
+        <v>57</v>
+      </c>
+      <c r="K2" t="s">
+        <v>58</v>
+      </c>
+      <c r="L2" t="s">
+        <v>59</v>
+      </c>
+      <c r="M2" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -855,235 +1001,54 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O6"/>
+  <dimension ref="B1:O1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="2:15">
       <c r="B1" s="1" t="s">
-        <v>44</v>
+        <v>61</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>45</v>
+        <v>62</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>46</v>
+        <v>63</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>47</v>
+        <v>64</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>48</v>
+        <v>65</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>49</v>
+        <v>66</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>50</v>
+        <v>67</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>51</v>
+        <v>68</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>52</v>
+        <v>69</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>53</v>
+        <v>70</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>54</v>
+        <v>71</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>55</v>
+        <v>72</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>56</v>
+        <v>73</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15">
-      <c r="A2" s="1">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>58</v>
-      </c>
-      <c r="C2" t="s">
-        <v>61</v>
-      </c>
-      <c r="D2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" t="s">
-        <v>69</v>
-      </c>
-      <c r="G2" t="s">
-        <v>71</v>
-      </c>
-      <c r="H2" t="s">
-        <v>69</v>
-      </c>
-      <c r="I2" t="s">
         <v>74</v>
-      </c>
-      <c r="N2" t="s">
-        <v>76</v>
-      </c>
-      <c r="O2" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15">
-      <c r="A3" s="1">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C3" t="s">
-        <v>62</v>
-      </c>
-      <c r="D3" t="s">
-        <v>66</v>
-      </c>
-      <c r="E3" t="s">
-        <v>67</v>
-      </c>
-      <c r="F3" t="s">
-        <v>68</v>
-      </c>
-      <c r="G3" t="s">
-        <v>72</v>
-      </c>
-      <c r="H3" t="s">
-        <v>67</v>
-      </c>
-      <c r="I3" t="s">
-        <v>74</v>
-      </c>
-      <c r="N3" t="s">
-        <v>77</v>
-      </c>
-      <c r="O3" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15">
-      <c r="A4" s="1">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>58</v>
-      </c>
-      <c r="C4" t="s">
-        <v>63</v>
-      </c>
-      <c r="D4" t="s">
-        <v>33</v>
-      </c>
-      <c r="E4" t="s">
-        <v>68</v>
-      </c>
-      <c r="F4" t="s">
-        <v>68</v>
-      </c>
-      <c r="G4" t="s">
-        <v>67</v>
-      </c>
-      <c r="H4" t="s">
-        <v>73</v>
-      </c>
-      <c r="I4" t="s">
-        <v>75</v>
-      </c>
-      <c r="J4" t="s">
-        <v>68</v>
-      </c>
-      <c r="K4" t="s">
-        <v>68</v>
-      </c>
-      <c r="N4" t="s">
-        <v>77</v>
-      </c>
-      <c r="O4" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15">
-      <c r="A5" s="1">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
-        <v>60</v>
-      </c>
-      <c r="C5" t="s">
-        <v>64</v>
-      </c>
-      <c r="D5" t="s">
-        <v>66</v>
-      </c>
-      <c r="E5" t="s">
-        <v>69</v>
-      </c>
-      <c r="F5" t="s">
-        <v>68</v>
-      </c>
-      <c r="G5" t="s">
-        <v>11</v>
-      </c>
-      <c r="H5" t="s">
-        <v>71</v>
-      </c>
-      <c r="I5" t="s">
-        <v>74</v>
-      </c>
-      <c r="N5" t="s">
-        <v>78</v>
-      </c>
-      <c r="O5" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15">
-      <c r="A6" s="1">
-        <v>4</v>
-      </c>
-      <c r="B6" t="s">
-        <v>58</v>
-      </c>
-      <c r="C6" t="s">
-        <v>65</v>
-      </c>
-      <c r="D6" t="s">
-        <v>33</v>
-      </c>
-      <c r="E6" t="s">
-        <v>67</v>
-      </c>
-      <c r="F6" t="s">
-        <v>70</v>
-      </c>
-      <c r="G6" t="s">
-        <v>11</v>
-      </c>
-      <c r="H6" t="s">
-        <v>70</v>
-      </c>
-      <c r="I6" t="s">
-        <v>74</v>
-      </c>
-      <c r="N6" t="s">
-        <v>77</v>
-      </c>
-      <c r="O6" t="s">
-        <v>79</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added session management constraints for all routes
</commit_message>
<xml_diff>
--- a/Event.xlsx
+++ b/Event.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="85">
   <si>
     <t>event_name</t>
   </si>
@@ -151,7 +151,7 @@
     <t>Cloud</t>
   </si>
   <si>
-    <t>[['Mr. Aditya', 'ISL']]</t>
+    <t>[['Mr. Aditya', 'ISL'], ['Mr. Manoj', 'GBS'], ['Dr. Dilip', 'GTS']]</t>
   </si>
   <si>
     <t>[['Dr. Dilip', 'ISL'], ['Dr. Aman', 'IRL'], ['Mr. Madhu', 'GBS'], ['Ms. Aditi', 'GTS']]</t>
@@ -187,13 +187,19 @@
     <t>box_location_feed</t>
   </si>
   <si>
-    <t xml:space="preserve">AI For Everyone </t>
-  </si>
-  <si>
-    <t>GBS</t>
-  </si>
-  <si>
-    <t>SME_NAME</t>
+    <t>tech sess 1</t>
+  </si>
+  <si>
+    <t>200000</t>
+  </si>
+  <si>
+    <t>2020-10-31</t>
+  </si>
+  <si>
+    <t>ISL</t>
+  </si>
+  <si>
+    <t>SME_NAME_2</t>
   </si>
   <si>
     <t>BOX LOC ATTENDEE</t>
@@ -242,6 +248,30 @@
   </si>
   <si>
     <t>project_url</t>
+  </si>
+  <si>
+    <t>ABC</t>
+  </si>
+  <si>
+    <t>tech #1</t>
+  </si>
+  <si>
+    <t>2020-11-01</t>
+  </si>
+  <si>
+    <t>Approved</t>
+  </si>
+  <si>
+    <t>Springer</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>SUR CITY</t>
+  </si>
+  <si>
+    <t>aSCHAJK</t>
   </si>
 </sst>
 </file>
@@ -964,34 +994,34 @@
         <v>56</v>
       </c>
       <c r="D2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E2" t="s">
-        <v>33</v>
+        <v>57</v>
       </c>
       <c r="F2" t="s">
-        <v>47</v>
+        <v>16</v>
       </c>
       <c r="G2" t="s">
-        <v>14</v>
+        <v>58</v>
       </c>
       <c r="H2" t="s">
-        <v>13</v>
+        <v>58</v>
       </c>
       <c r="I2" t="s">
         <v>41</v>
       </c>
       <c r="J2" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="K2" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="L2" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="M2" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -1001,54 +1031,101 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:O1"/>
+  <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="2:15">
+    <row r="1" spans="1:15">
       <c r="B1" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>74</v>
+        <v>76</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D2" t="s">
+        <v>78</v>
+      </c>
+      <c r="E2" t="s">
+        <v>79</v>
+      </c>
+      <c r="F2" t="s">
+        <v>79</v>
+      </c>
+      <c r="G2" t="s">
+        <v>79</v>
+      </c>
+      <c r="H2" t="s">
+        <v>79</v>
+      </c>
+      <c r="I2" t="s">
+        <v>80</v>
+      </c>
+      <c r="J2" t="s">
+        <v>79</v>
+      </c>
+      <c r="K2" t="s">
+        <v>79</v>
+      </c>
+      <c r="L2" t="s">
+        <v>81</v>
+      </c>
+      <c r="M2" t="s">
+        <v>82</v>
+      </c>
+      <c r="N2" t="s">
+        <v>83</v>
+      </c>
+      <c r="O2" t="s">
+        <v>84</v>
       </c>
     </row>
   </sheetData>

</xml_diff>